<commit_message>
clean up dates and opmerkingen
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2022_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_VA_2022_2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Maart 2022" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5446" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5439" uniqueCount="66">
   <si>
     <t>Waterpeil aanpassingen Veurne - Ambacht</t>
   </si>
@@ -988,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L320"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3096,7 +3096,9 @@
       <c r="H96" s="32"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A97" s="23"/>
+      <c r="A97" s="23">
+        <v>44631</v>
+      </c>
       <c r="B97" s="24">
         <v>0.15625</v>
       </c>
@@ -3120,9 +3122,6 @@
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A98" s="23">
-        <v>44631</v>
-      </c>
       <c r="B98" s="24">
         <v>0.33333333333333331</v>
       </c>
@@ -6860,9 +6859,7 @@
       <c r="G266" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="H266" s="29" t="s">
-        <v>49</v>
-      </c>
+      <c r="H266" s="29"/>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A267" s="23">
@@ -7708,6 +7705,7 @@
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7715,8 +7713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B124" sqref="B124"/>
+    <sheetView topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="I251" sqref="I251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14470,8 +14468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L317"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15242,7 +15240,7 @@
         <v>44685</v>
       </c>
       <c r="B37" s="24">
-        <v>2.52</v>
+        <v>2.02</v>
       </c>
       <c r="C37" s="25">
         <v>2.13</v>
@@ -20221,8 +20219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L318"/>
   <sheetViews>
-    <sheetView topLeftCell="A278" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="C158" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20358,9 +20356,7 @@
       <c r="G8" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="23"/>
@@ -20560,7 +20556,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="23">
-        <v>44960</v>
+        <v>44988</v>
       </c>
       <c r="B18" s="24">
         <v>3.125E-2</v>
@@ -23710,7 +23706,9 @@
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A160" s="23"/>
+      <c r="A160" s="23">
+        <v>45004</v>
+      </c>
       <c r="B160" s="24">
         <v>4.8611111111111112E-2</v>
       </c>
@@ -23732,9 +23730,6 @@
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A161" s="23">
-        <v>45004</v>
-      </c>
       <c r="B161" s="24">
         <v>0.16666666666666666</v>
       </c>
@@ -26940,10 +26935,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L320"/>
+  <dimension ref="A1:L319"/>
   <sheetViews>
-    <sheetView topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="H231" sqref="H231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27481,9 +27476,7 @@
       <c r="G26" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="50" t="s">
-        <v>15</v>
-      </c>
+      <c r="H26" s="50"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="23"/>
@@ -29691,7 +29684,9 @@
       <c r="G125" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="H125" s="50"/>
+      <c r="H125" s="50" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="23">
@@ -31028,9 +31023,7 @@
       <c r="G185" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="H185" s="51" t="s">
-        <v>15</v>
-      </c>
+      <c r="H185" s="51"/>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186" s="23">
@@ -31455,7 +31448,9 @@
       <c r="H204" s="51"/>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A205" s="23"/>
+      <c r="A205" s="23">
+        <v>45039</v>
+      </c>
       <c r="B205" s="24">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -31501,9 +31496,6 @@
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A207" s="23">
-        <v>45039</v>
-      </c>
       <c r="B207" s="24">
         <v>0.23958333333333334</v>
       </c>
@@ -32011,7 +32003,7 @@
         <v>13</v>
       </c>
       <c r="H229" s="51" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.35">
@@ -32902,27 +32894,17 @@
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A270" s="23"/>
-      <c r="B270" s="24">
-        <v>6.9444444444444434E-2</v>
-      </c>
-      <c r="C270" s="25">
-        <v>2.7</v>
-      </c>
+      <c r="B270" s="24"/>
+      <c r="C270" s="25"/>
       <c r="D270" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E270" s="27">
-        <v>2.7</v>
-      </c>
+      <c r="E270" s="27"/>
       <c r="F270" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G270" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="H270" s="51" t="s">
-        <v>15</v>
-      </c>
+      <c r="G270" s="31"/>
+      <c r="H270" s="51"/>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A271" s="23"/>
@@ -33025,7 +33007,7 @@
     <row r="278" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A278" s="23"/>
       <c r="B278" s="24"/>
-      <c r="C278" s="25"/>
+      <c r="C278" s="39"/>
       <c r="D278" s="26" t="s">
         <v>10</v>
       </c>
@@ -33033,13 +33015,13 @@
       <c r="F278" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G278" s="31"/>
+      <c r="G278" s="38"/>
       <c r="H278" s="51"/>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A279" s="23"/>
       <c r="B279" s="24"/>
-      <c r="C279" s="39"/>
+      <c r="C279" s="25"/>
       <c r="D279" s="26" t="s">
         <v>10</v>
       </c>
@@ -33047,7 +33029,7 @@
       <c r="F279" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G279" s="38"/>
+      <c r="G279" s="31"/>
       <c r="H279" s="51"/>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.35">
@@ -33159,7 +33141,7 @@
       <c r="F287" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G287" s="31"/>
+      <c r="G287" s="38"/>
       <c r="H287" s="51"/>
     </row>
     <row r="288" spans="1:8" x14ac:dyDescent="0.35">
@@ -33333,11 +33315,11 @@
     <row r="300" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A300" s="23"/>
       <c r="B300" s="24"/>
-      <c r="C300" s="25"/>
+      <c r="C300" s="39"/>
       <c r="D300" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E300" s="27"/>
+      <c r="E300" s="42"/>
       <c r="F300" s="26" t="s">
         <v>10</v>
       </c>
@@ -33347,15 +33329,15 @@
     <row r="301" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A301" s="23"/>
       <c r="B301" s="24"/>
-      <c r="C301" s="39"/>
+      <c r="C301" s="25"/>
       <c r="D301" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E301" s="42"/>
+      <c r="E301" s="27"/>
       <c r="F301" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G301" s="38"/>
+      <c r="G301" s="31"/>
       <c r="H301" s="51"/>
     </row>
     <row r="302" spans="1:8" x14ac:dyDescent="0.35">
@@ -33398,7 +33380,7 @@
         <v>10</v>
       </c>
       <c r="G304" s="31"/>
-      <c r="H304" s="51"/>
+      <c r="H304" s="50"/>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A305" s="23"/>
@@ -33529,7 +33511,7 @@
     <row r="314" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A314" s="23"/>
       <c r="B314" s="24"/>
-      <c r="C314" s="25"/>
+      <c r="C314" s="39"/>
       <c r="D314" s="26" t="s">
         <v>10</v>
       </c>
@@ -33543,7 +33525,7 @@
     <row r="315" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A315" s="23"/>
       <c r="B315" s="24"/>
-      <c r="C315" s="39"/>
+      <c r="C315" s="25"/>
       <c r="D315" s="26" t="s">
         <v>10</v>
       </c>
@@ -33609,20 +33591,6 @@
       </c>
       <c r="G319" s="31"/>
       <c r="H319" s="50"/>
-    </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A320" s="23"/>
-      <c r="B320" s="24"/>
-      <c r="C320" s="25"/>
-      <c r="D320" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E320" s="27"/>
-      <c r="F320" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G320" s="31"/>
-      <c r="H320" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -33630,6 +33598,7 @@
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -33637,8 +33606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L318"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33756,7 +33725,9 @@
       <c r="G7" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="29"/>
+      <c r="H7" s="51" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="23"/>
@@ -33893,7 +33864,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="23"/>
+      <c r="A14" s="23">
+        <v>45048</v>
+      </c>
       <c r="B14" s="24">
         <v>0.1111111111111111</v>
       </c>
@@ -33917,9 +33890,6 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="23">
-        <v>45048</v>
-      </c>
       <c r="B15" s="24">
         <v>0.19097222222222221</v>
       </c>
@@ -34923,9 +34893,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A60" s="23">
-        <v>45053</v>
-      </c>
+      <c r="A60" s="23"/>
       <c r="B60" s="24">
         <v>0.25</v>
       </c>
@@ -34966,9 +34934,7 @@
       <c r="G61" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="H61" s="32" t="s">
-        <v>44</v>
-      </c>
+      <c r="H61" s="32"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="23"/>

</xml_diff>